<commit_message>
excel uploading and reading data success
</commit_message>
<xml_diff>
--- a/uploads/test.xlsx
+++ b/uploads/test.xlsx
@@ -33,28 +33,28 @@
     <t>student_college_id</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Eldhose</t>
-  </si>
-  <si>
-    <t>Abhinand</t>
-  </si>
-  <si>
-    <t>Amir</t>
-  </si>
-  <si>
-    <t>alex@gmail.com</t>
-  </si>
-  <si>
-    <t>eldhose@gmail.com</t>
-  </si>
-  <si>
-    <t>abhinand@gmail.com</t>
-  </si>
-  <si>
-    <t>amir@gmail.com</t>
+    <t>Anex</t>
+  </si>
+  <si>
+    <t>anex@gmail.com</t>
+  </si>
+  <si>
+    <t>Jeffin</t>
+  </si>
+  <si>
+    <t>jeffin@gmail.com</t>
+  </si>
+  <si>
+    <t>Mahadevan</t>
+  </si>
+  <si>
+    <t>Melvin</t>
+  </si>
+  <si>
+    <t>Melvin@gmail.com</t>
+  </si>
+  <si>
+    <t>mahadevan@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -103,14 +103,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,91 +443,95 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4">
-        <v>862</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5">
+        <v>1522</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4"/>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4">
-        <v>1256</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3"/>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5">
+        <v>9638</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="4">
-        <v>2541</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="C4" s="5">
+        <v>7531</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
         <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="5">
-        <v>458</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3"/>
+      <c r="C5" s="6">
+        <v>5548</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
         <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
       </c>
       <c r="I5" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
@@ -544,10 +548,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>

</xml_diff>